<commit_message>
fix loi neu co
</commit_message>
<xml_diff>
--- a/public/baoCaoXNT/06_2024.xlsx
+++ b/public/baoCaoXNT/06_2024.xlsx
@@ -599,18 +599,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="true" style="0"/>
-    <col min="2" max="2" width="70" customWidth="true" style="0"/>
+    <col min="1" max="1" width="10" customWidth="true" style="0"/>
+    <col min="2" max="2" width="60" customWidth="true" style="0"/>
     <col min="3" max="3" width="5" hidden="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="15" customWidth="true" style="0"/>
-    <col min="5" max="5" width="15" customWidth="true" style="0"/>
-    <col min="6" max="6" width="15" customWidth="true" style="0"/>
+    <col min="4" max="4" width="10" customWidth="true" style="0"/>
+    <col min="5" max="5" width="10" customWidth="true" style="0"/>
+    <col min="6" max="6" width="12" customWidth="true" style="0"/>
     <col min="7" max="7" width="15" customWidth="true" style="0"/>
-    <col min="8" max="8" width="15" customWidth="true" style="0"/>
-    <col min="9" max="9" width="15" customWidth="true" style="0"/>
+    <col min="8" max="8" width="10" customWidth="true" style="0"/>
+    <col min="9" max="9" width="12" customWidth="true" style="0"/>
     <col min="10" max="10" width="15" customWidth="true" style="0"/>
-    <col min="11" max="11" width="15" customWidth="true" style="0"/>
-    <col min="12" max="12" width="15" customWidth="true" style="0"/>
+    <col min="11" max="11" width="10" customWidth="true" style="0"/>
+    <col min="12" max="12" width="12" customWidth="true" style="0"/>
     <col min="13" max="13" width="15" customWidth="true" style="0"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
bao cao doanh thu xuat file
</commit_message>
<xml_diff>
--- a/public/baoCaoXNT/06_2024.xlsx
+++ b/public/baoCaoXNT/06_2024.xlsx
@@ -266,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
@@ -284,6 +284,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="5" numFmtId="0" fillId="3" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="3" fillId="0" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="5" numFmtId="3" fillId="3" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="4" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
@@ -653,7 +659,7 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" customHeight="1" ht="30">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -728,31 +734,31 @@
       <c r="D7" s="5">
         <v>3</v>
       </c>
-      <c r="E7" s="5">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5">
+      <c r="E7" s="7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7">
         <v>14990000</v>
       </c>
-      <c r="G7" s="5">
-        <v>0</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0</v>
-      </c>
-      <c r="I7" s="5">
+      <c r="G7" s="7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7">
         <v>14990000</v>
       </c>
-      <c r="J7" s="5">
-        <v>0</v>
-      </c>
-      <c r="K7" s="5">
+      <c r="J7" s="7">
+        <v>0</v>
+      </c>
+      <c r="K7" s="7">
         <v>3</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="7">
         <v>14990000</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="7">
         <v>44970000</v>
       </c>
     </row>
@@ -769,31 +775,31 @@
       <c r="D8" s="5">
         <v>10</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="7">
         <v>2</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="7">
         <v>1300000</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="7">
         <v>2600000</v>
       </c>
-      <c r="H8" s="5">
-        <v>0</v>
-      </c>
-      <c r="I8" s="5">
+      <c r="H8" s="7">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7">
         <v>5490000</v>
       </c>
-      <c r="J8" s="5">
-        <v>0</v>
-      </c>
-      <c r="K8" s="5">
+      <c r="J8" s="7">
+        <v>0</v>
+      </c>
+      <c r="K8" s="7">
         <v>12</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="7">
         <v>5490000</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="7">
         <v>65880000</v>
       </c>
     </row>
@@ -810,31 +816,31 @@
       <c r="D9" s="5">
         <v>10</v>
       </c>
-      <c r="E9" s="5">
-        <v>0</v>
-      </c>
-      <c r="F9" s="5">
+      <c r="E9" s="7">
+        <v>0</v>
+      </c>
+      <c r="F9" s="7">
         <v>14590000</v>
       </c>
-      <c r="G9" s="5">
-        <v>0</v>
-      </c>
-      <c r="H9" s="5">
-        <v>0</v>
-      </c>
-      <c r="I9" s="5">
+      <c r="G9" s="7">
+        <v>0</v>
+      </c>
+      <c r="H9" s="7">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7">
         <v>14590000</v>
       </c>
-      <c r="J9" s="5">
-        <v>0</v>
-      </c>
-      <c r="K9" s="5">
-        <v>10</v>
-      </c>
-      <c r="L9" s="5">
+      <c r="J9" s="7">
+        <v>0</v>
+      </c>
+      <c r="K9" s="7">
+        <v>10</v>
+      </c>
+      <c r="L9" s="7">
         <v>14590000</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="7">
         <v>145900000</v>
       </c>
     </row>
@@ -851,31 +857,31 @@
       <c r="D10" s="5">
         <v>10</v>
       </c>
-      <c r="E10" s="5">
-        <v>0</v>
-      </c>
-      <c r="F10" s="5">
+      <c r="E10" s="7">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7">
         <v>11990000</v>
       </c>
-      <c r="G10" s="5">
-        <v>0</v>
-      </c>
-      <c r="H10" s="5">
-        <v>0</v>
-      </c>
-      <c r="I10" s="5">
+      <c r="G10" s="7">
+        <v>0</v>
+      </c>
+      <c r="H10" s="7">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7">
         <v>11990000</v>
       </c>
-      <c r="J10" s="5">
-        <v>0</v>
-      </c>
-      <c r="K10" s="5">
-        <v>10</v>
-      </c>
-      <c r="L10" s="5">
+      <c r="J10" s="7">
+        <v>0</v>
+      </c>
+      <c r="K10" s="7">
+        <v>10</v>
+      </c>
+      <c r="L10" s="7">
         <v>11990000</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10" s="7">
         <v>119900000</v>
       </c>
     </row>
@@ -892,31 +898,31 @@
       <c r="D11" s="5">
         <v>10</v>
       </c>
-      <c r="E11" s="5">
-        <v>0</v>
-      </c>
-      <c r="F11" s="5">
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7">
         <v>14990000</v>
       </c>
-      <c r="G11" s="5">
-        <v>0</v>
-      </c>
-      <c r="H11" s="5">
-        <v>0</v>
-      </c>
-      <c r="I11" s="5">
+      <c r="G11" s="7">
+        <v>0</v>
+      </c>
+      <c r="H11" s="7">
+        <v>0</v>
+      </c>
+      <c r="I11" s="7">
         <v>14990000</v>
       </c>
-      <c r="J11" s="5">
-        <v>0</v>
-      </c>
-      <c r="K11" s="5">
-        <v>10</v>
-      </c>
-      <c r="L11" s="5">
+      <c r="J11" s="7">
+        <v>0</v>
+      </c>
+      <c r="K11" s="7">
+        <v>10</v>
+      </c>
+      <c r="L11" s="7">
         <v>14990000</v>
       </c>
-      <c r="M11" s="5">
+      <c r="M11" s="7">
         <v>149900000</v>
       </c>
     </row>
@@ -933,31 +939,31 @@
       <c r="D12" s="5">
         <v>10</v>
       </c>
-      <c r="E12" s="5">
-        <v>0</v>
-      </c>
-      <c r="F12" s="5">
+      <c r="E12" s="7">
+        <v>0</v>
+      </c>
+      <c r="F12" s="7">
         <v>20490000</v>
       </c>
-      <c r="G12" s="5">
-        <v>0</v>
-      </c>
-      <c r="H12" s="5">
-        <v>0</v>
-      </c>
-      <c r="I12" s="5">
+      <c r="G12" s="7">
+        <v>0</v>
+      </c>
+      <c r="H12" s="7">
+        <v>0</v>
+      </c>
+      <c r="I12" s="7">
         <v>20490000</v>
       </c>
-      <c r="J12" s="5">
-        <v>0</v>
-      </c>
-      <c r="K12" s="5">
-        <v>10</v>
-      </c>
-      <c r="L12" s="5">
+      <c r="J12" s="7">
+        <v>0</v>
+      </c>
+      <c r="K12" s="7">
+        <v>10</v>
+      </c>
+      <c r="L12" s="7">
         <v>20490000</v>
       </c>
-      <c r="M12" s="5">
+      <c r="M12" s="7">
         <v>204900000</v>
       </c>
     </row>
@@ -974,31 +980,31 @@
       <c r="D13" s="5">
         <v>10</v>
       </c>
-      <c r="E13" s="5">
-        <v>0</v>
-      </c>
-      <c r="F13" s="5">
+      <c r="E13" s="7">
+        <v>0</v>
+      </c>
+      <c r="F13" s="7">
         <v>24990000</v>
       </c>
-      <c r="G13" s="5">
-        <v>0</v>
-      </c>
-      <c r="H13" s="5">
-        <v>0</v>
-      </c>
-      <c r="I13" s="5">
+      <c r="G13" s="7">
+        <v>0</v>
+      </c>
+      <c r="H13" s="7">
+        <v>0</v>
+      </c>
+      <c r="I13" s="7">
         <v>24990000</v>
       </c>
-      <c r="J13" s="5">
-        <v>0</v>
-      </c>
-      <c r="K13" s="5">
-        <v>10</v>
-      </c>
-      <c r="L13" s="5">
+      <c r="J13" s="7">
+        <v>0</v>
+      </c>
+      <c r="K13" s="7">
+        <v>10</v>
+      </c>
+      <c r="L13" s="7">
         <v>24990000</v>
       </c>
-      <c r="M13" s="5">
+      <c r="M13" s="7">
         <v>249900000</v>
       </c>
     </row>
@@ -1015,31 +1021,31 @@
       <c r="D14" s="5">
         <v>10</v>
       </c>
-      <c r="E14" s="5">
-        <v>0</v>
-      </c>
-      <c r="F14" s="5">
+      <c r="E14" s="7">
+        <v>0</v>
+      </c>
+      <c r="F14" s="7">
         <v>4990000</v>
       </c>
-      <c r="G14" s="5">
-        <v>0</v>
-      </c>
-      <c r="H14" s="5">
-        <v>0</v>
-      </c>
-      <c r="I14" s="5">
+      <c r="G14" s="7">
+        <v>0</v>
+      </c>
+      <c r="H14" s="7">
+        <v>0</v>
+      </c>
+      <c r="I14" s="7">
         <v>4990000</v>
       </c>
-      <c r="J14" s="5">
-        <v>0</v>
-      </c>
-      <c r="K14" s="5">
-        <v>10</v>
-      </c>
-      <c r="L14" s="5">
+      <c r="J14" s="7">
+        <v>0</v>
+      </c>
+      <c r="K14" s="7">
+        <v>10</v>
+      </c>
+      <c r="L14" s="7">
         <v>4990000</v>
       </c>
-      <c r="M14" s="5">
+      <c r="M14" s="7">
         <v>49900000</v>
       </c>
     </row>
@@ -1056,31 +1062,31 @@
       <c r="D15" s="5">
         <v>10</v>
       </c>
-      <c r="E15" s="5">
-        <v>0</v>
-      </c>
-      <c r="F15" s="5">
+      <c r="E15" s="7">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7">
         <v>29590000</v>
       </c>
-      <c r="G15" s="5">
-        <v>0</v>
-      </c>
-      <c r="H15" s="5">
-        <v>0</v>
-      </c>
-      <c r="I15" s="5">
+      <c r="G15" s="7">
+        <v>0</v>
+      </c>
+      <c r="H15" s="7">
+        <v>0</v>
+      </c>
+      <c r="I15" s="7">
         <v>29590000</v>
       </c>
-      <c r="J15" s="5">
-        <v>0</v>
-      </c>
-      <c r="K15" s="5">
-        <v>10</v>
-      </c>
-      <c r="L15" s="5">
+      <c r="J15" s="7">
+        <v>0</v>
+      </c>
+      <c r="K15" s="7">
+        <v>10</v>
+      </c>
+      <c r="L15" s="7">
         <v>29590000</v>
       </c>
-      <c r="M15" s="5">
+      <c r="M15" s="7">
         <v>295900000</v>
       </c>
     </row>
@@ -1097,31 +1103,31 @@
       <c r="D16" s="5">
         <v>10</v>
       </c>
-      <c r="E16" s="5">
-        <v>0</v>
-      </c>
-      <c r="F16" s="5">
+      <c r="E16" s="7">
+        <v>0</v>
+      </c>
+      <c r="F16" s="7">
         <v>7990000</v>
       </c>
-      <c r="G16" s="5">
-        <v>0</v>
-      </c>
-      <c r="H16" s="5">
-        <v>0</v>
-      </c>
-      <c r="I16" s="5">
+      <c r="G16" s="7">
+        <v>0</v>
+      </c>
+      <c r="H16" s="7">
+        <v>0</v>
+      </c>
+      <c r="I16" s="7">
         <v>7990000</v>
       </c>
-      <c r="J16" s="5">
-        <v>0</v>
-      </c>
-      <c r="K16" s="5">
-        <v>10</v>
-      </c>
-      <c r="L16" s="5">
+      <c r="J16" s="7">
+        <v>0</v>
+      </c>
+      <c r="K16" s="7">
+        <v>10</v>
+      </c>
+      <c r="L16" s="7">
         <v>7990000</v>
       </c>
-      <c r="M16" s="5">
+      <c r="M16" s="7">
         <v>79900000</v>
       </c>
     </row>
@@ -1138,31 +1144,31 @@
       <c r="D17" s="5">
         <v>10</v>
       </c>
-      <c r="E17" s="5">
-        <v>0</v>
-      </c>
-      <c r="F17" s="5">
+      <c r="E17" s="7">
+        <v>0</v>
+      </c>
+      <c r="F17" s="7">
         <v>4990000</v>
       </c>
-      <c r="G17" s="5">
-        <v>0</v>
-      </c>
-      <c r="H17" s="5">
-        <v>0</v>
-      </c>
-      <c r="I17" s="5">
+      <c r="G17" s="7">
+        <v>0</v>
+      </c>
+      <c r="H17" s="7">
+        <v>0</v>
+      </c>
+      <c r="I17" s="7">
         <v>4990000</v>
       </c>
-      <c r="J17" s="5">
-        <v>0</v>
-      </c>
-      <c r="K17" s="5">
-        <v>10</v>
-      </c>
-      <c r="L17" s="5">
+      <c r="J17" s="7">
+        <v>0</v>
+      </c>
+      <c r="K17" s="7">
+        <v>10</v>
+      </c>
+      <c r="L17" s="7">
         <v>4990000</v>
       </c>
-      <c r="M17" s="5">
+      <c r="M17" s="7">
         <v>49900000</v>
       </c>
     </row>
@@ -1179,31 +1185,31 @@
       <c r="D18" s="5">
         <v>10</v>
       </c>
-      <c r="E18" s="5">
-        <v>0</v>
-      </c>
-      <c r="F18" s="5">
+      <c r="E18" s="7">
+        <v>0</v>
+      </c>
+      <c r="F18" s="7">
         <v>6890000</v>
       </c>
-      <c r="G18" s="5">
-        <v>0</v>
-      </c>
-      <c r="H18" s="5">
-        <v>0</v>
-      </c>
-      <c r="I18" s="5">
+      <c r="G18" s="7">
+        <v>0</v>
+      </c>
+      <c r="H18" s="7">
+        <v>0</v>
+      </c>
+      <c r="I18" s="7">
         <v>6890000</v>
       </c>
-      <c r="J18" s="5">
-        <v>0</v>
-      </c>
-      <c r="K18" s="5">
-        <v>10</v>
-      </c>
-      <c r="L18" s="5">
+      <c r="J18" s="7">
+        <v>0</v>
+      </c>
+      <c r="K18" s="7">
+        <v>10</v>
+      </c>
+      <c r="L18" s="7">
         <v>6890000</v>
       </c>
-      <c r="M18" s="5">
+      <c r="M18" s="7">
         <v>68900000</v>
       </c>
     </row>
@@ -1220,31 +1226,31 @@
       <c r="D19" s="5">
         <v>8</v>
       </c>
-      <c r="E19" s="5">
-        <v>0</v>
-      </c>
-      <c r="F19" s="5">
+      <c r="E19" s="7">
+        <v>0</v>
+      </c>
+      <c r="F19" s="7">
         <v>5990000</v>
       </c>
-      <c r="G19" s="5">
-        <v>0</v>
-      </c>
-      <c r="H19" s="5">
-        <v>0</v>
-      </c>
-      <c r="I19" s="5">
+      <c r="G19" s="7">
+        <v>0</v>
+      </c>
+      <c r="H19" s="7">
+        <v>0</v>
+      </c>
+      <c r="I19" s="7">
         <v>5990000</v>
       </c>
-      <c r="J19" s="5">
-        <v>0</v>
-      </c>
-      <c r="K19" s="5">
+      <c r="J19" s="7">
+        <v>0</v>
+      </c>
+      <c r="K19" s="7">
         <v>8</v>
       </c>
-      <c r="L19" s="5">
+      <c r="L19" s="7">
         <v>5990000</v>
       </c>
-      <c r="M19" s="5">
+      <c r="M19" s="7">
         <v>47920000</v>
       </c>
     </row>
@@ -1261,31 +1267,31 @@
       <c r="D20" s="5">
         <v>10</v>
       </c>
-      <c r="E20" s="5">
-        <v>0</v>
-      </c>
-      <c r="F20" s="5">
+      <c r="E20" s="7">
+        <v>0</v>
+      </c>
+      <c r="F20" s="7">
         <v>39490000</v>
       </c>
-      <c r="G20" s="5">
-        <v>0</v>
-      </c>
-      <c r="H20" s="5">
-        <v>0</v>
-      </c>
-      <c r="I20" s="5">
+      <c r="G20" s="7">
+        <v>0</v>
+      </c>
+      <c r="H20" s="7">
+        <v>0</v>
+      </c>
+      <c r="I20" s="7">
         <v>39490000</v>
       </c>
-      <c r="J20" s="5">
-        <v>0</v>
-      </c>
-      <c r="K20" s="5">
-        <v>10</v>
-      </c>
-      <c r="L20" s="5">
+      <c r="J20" s="7">
+        <v>0</v>
+      </c>
+      <c r="K20" s="7">
+        <v>10</v>
+      </c>
+      <c r="L20" s="7">
         <v>39490000</v>
       </c>
-      <c r="M20" s="5">
+      <c r="M20" s="7">
         <v>394900000</v>
       </c>
     </row>
@@ -1302,31 +1308,31 @@
       <c r="D21" s="5">
         <v>10</v>
       </c>
-      <c r="E21" s="5">
-        <v>0</v>
-      </c>
-      <c r="F21" s="5">
+      <c r="E21" s="7">
+        <v>0</v>
+      </c>
+      <c r="F21" s="7">
         <v>29690000</v>
       </c>
-      <c r="G21" s="5">
-        <v>0</v>
-      </c>
-      <c r="H21" s="5">
-        <v>0</v>
-      </c>
-      <c r="I21" s="5">
+      <c r="G21" s="7">
+        <v>0</v>
+      </c>
+      <c r="H21" s="7">
+        <v>0</v>
+      </c>
+      <c r="I21" s="7">
         <v>29690000</v>
       </c>
-      <c r="J21" s="5">
-        <v>0</v>
-      </c>
-      <c r="K21" s="5">
-        <v>10</v>
-      </c>
-      <c r="L21" s="5">
+      <c r="J21" s="7">
+        <v>0</v>
+      </c>
+      <c r="K21" s="7">
+        <v>10</v>
+      </c>
+      <c r="L21" s="7">
         <v>29690000</v>
       </c>
-      <c r="M21" s="5">
+      <c r="M21" s="7">
         <v>296900000</v>
       </c>
     </row>
@@ -1343,31 +1349,31 @@
       <c r="D22" s="5">
         <v>10</v>
       </c>
-      <c r="E22" s="5">
-        <v>0</v>
-      </c>
-      <c r="F22" s="5">
+      <c r="E22" s="7">
+        <v>0</v>
+      </c>
+      <c r="F22" s="7">
         <v>10990000</v>
       </c>
-      <c r="G22" s="5">
-        <v>0</v>
-      </c>
-      <c r="H22" s="5">
-        <v>0</v>
-      </c>
-      <c r="I22" s="5">
+      <c r="G22" s="7">
+        <v>0</v>
+      </c>
+      <c r="H22" s="7">
+        <v>0</v>
+      </c>
+      <c r="I22" s="7">
         <v>10990000</v>
       </c>
-      <c r="J22" s="5">
-        <v>0</v>
-      </c>
-      <c r="K22" s="5">
-        <v>10</v>
-      </c>
-      <c r="L22" s="5">
+      <c r="J22" s="7">
+        <v>0</v>
+      </c>
+      <c r="K22" s="7">
+        <v>10</v>
+      </c>
+      <c r="L22" s="7">
         <v>10990000</v>
       </c>
-      <c r="M22" s="5">
+      <c r="M22" s="7">
         <v>109900000</v>
       </c>
     </row>
@@ -1384,31 +1390,31 @@
       <c r="D23" s="5">
         <v>9</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="7">
         <v>3</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="7">
         <v>4000000</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="7">
         <v>12000000</v>
       </c>
-      <c r="H23" s="5">
-        <v>0</v>
-      </c>
-      <c r="I23" s="5">
+      <c r="H23" s="7">
+        <v>0</v>
+      </c>
+      <c r="I23" s="7">
         <v>5990000</v>
       </c>
-      <c r="J23" s="5">
-        <v>0</v>
-      </c>
-      <c r="K23" s="5">
+      <c r="J23" s="7">
+        <v>0</v>
+      </c>
+      <c r="K23" s="7">
         <v>12</v>
       </c>
-      <c r="L23" s="5">
+      <c r="L23" s="7">
         <v>5990000</v>
       </c>
-      <c r="M23" s="5">
+      <c r="M23" s="7">
         <v>71880000</v>
       </c>
     </row>
@@ -1425,31 +1431,31 @@
       <c r="D24" s="5">
         <v>8</v>
       </c>
-      <c r="E24" s="5">
-        <v>0</v>
-      </c>
-      <c r="F24" s="5">
+      <c r="E24" s="7">
+        <v>0</v>
+      </c>
+      <c r="F24" s="7">
         <v>6990000</v>
       </c>
-      <c r="G24" s="5">
-        <v>0</v>
-      </c>
-      <c r="H24" s="5">
-        <v>0</v>
-      </c>
-      <c r="I24" s="5">
+      <c r="G24" s="7">
+        <v>0</v>
+      </c>
+      <c r="H24" s="7">
+        <v>0</v>
+      </c>
+      <c r="I24" s="7">
         <v>6990000</v>
       </c>
-      <c r="J24" s="5">
-        <v>0</v>
-      </c>
-      <c r="K24" s="5">
+      <c r="J24" s="7">
+        <v>0</v>
+      </c>
+      <c r="K24" s="7">
         <v>8</v>
       </c>
-      <c r="L24" s="5">
+      <c r="L24" s="7">
         <v>6990000</v>
       </c>
-      <c r="M24" s="5">
+      <c r="M24" s="7">
         <v>55920000</v>
       </c>
     </row>
@@ -1466,31 +1472,31 @@
       <c r="D25" s="5">
         <v>10</v>
       </c>
-      <c r="E25" s="5">
-        <v>0</v>
-      </c>
-      <c r="F25" s="5">
+      <c r="E25" s="7">
+        <v>0</v>
+      </c>
+      <c r="F25" s="7">
         <v>8990000</v>
       </c>
-      <c r="G25" s="5">
-        <v>0</v>
-      </c>
-      <c r="H25" s="5">
-        <v>0</v>
-      </c>
-      <c r="I25" s="5">
+      <c r="G25" s="7">
+        <v>0</v>
+      </c>
+      <c r="H25" s="7">
+        <v>0</v>
+      </c>
+      <c r="I25" s="7">
         <v>8990000</v>
       </c>
-      <c r="J25" s="5">
-        <v>0</v>
-      </c>
-      <c r="K25" s="5">
-        <v>10</v>
-      </c>
-      <c r="L25" s="5">
+      <c r="J25" s="7">
+        <v>0</v>
+      </c>
+      <c r="K25" s="7">
+        <v>10</v>
+      </c>
+      <c r="L25" s="7">
         <v>8990000</v>
       </c>
-      <c r="M25" s="5">
+      <c r="M25" s="7">
         <v>89900000</v>
       </c>
     </row>
@@ -1507,31 +1513,31 @@
       <c r="D26" s="5">
         <v>10</v>
       </c>
-      <c r="E26" s="5">
-        <v>0</v>
-      </c>
-      <c r="F26" s="5">
+      <c r="E26" s="7">
+        <v>0</v>
+      </c>
+      <c r="F26" s="7">
         <v>16890000</v>
       </c>
-      <c r="G26" s="5">
-        <v>0</v>
-      </c>
-      <c r="H26" s="5">
-        <v>0</v>
-      </c>
-      <c r="I26" s="5">
+      <c r="G26" s="7">
+        <v>0</v>
+      </c>
+      <c r="H26" s="7">
+        <v>0</v>
+      </c>
+      <c r="I26" s="7">
         <v>16890000</v>
       </c>
-      <c r="J26" s="5">
-        <v>0</v>
-      </c>
-      <c r="K26" s="5">
-        <v>10</v>
-      </c>
-      <c r="L26" s="5">
+      <c r="J26" s="7">
+        <v>0</v>
+      </c>
+      <c r="K26" s="7">
+        <v>10</v>
+      </c>
+      <c r="L26" s="7">
         <v>16890000</v>
       </c>
-      <c r="M26" s="5">
+      <c r="M26" s="7">
         <v>168900000</v>
       </c>
     </row>
@@ -1548,31 +1554,31 @@
       <c r="D27" s="5">
         <v>8</v>
       </c>
-      <c r="E27" s="5">
-        <v>0</v>
-      </c>
-      <c r="F27" s="5">
+      <c r="E27" s="7">
+        <v>0</v>
+      </c>
+      <c r="F27" s="7">
         <v>7990000</v>
       </c>
-      <c r="G27" s="5">
-        <v>0</v>
-      </c>
-      <c r="H27" s="5">
-        <v>0</v>
-      </c>
-      <c r="I27" s="5">
+      <c r="G27" s="7">
+        <v>0</v>
+      </c>
+      <c r="H27" s="7">
+        <v>0</v>
+      </c>
+      <c r="I27" s="7">
         <v>7990000</v>
       </c>
-      <c r="J27" s="5">
-        <v>0</v>
-      </c>
-      <c r="K27" s="5">
+      <c r="J27" s="7">
+        <v>0</v>
+      </c>
+      <c r="K27" s="7">
         <v>8</v>
       </c>
-      <c r="L27" s="5">
+      <c r="L27" s="7">
         <v>7990000</v>
       </c>
-      <c r="M27" s="5">
+      <c r="M27" s="7">
         <v>63920000</v>
       </c>
     </row>
@@ -1589,31 +1595,31 @@
       <c r="D28" s="5">
         <v>9</v>
       </c>
-      <c r="E28" s="5">
-        <v>0</v>
-      </c>
-      <c r="F28" s="5">
+      <c r="E28" s="7">
+        <v>0</v>
+      </c>
+      <c r="F28" s="7">
         <v>10490000</v>
       </c>
-      <c r="G28" s="5">
-        <v>0</v>
-      </c>
-      <c r="H28" s="5">
-        <v>0</v>
-      </c>
-      <c r="I28" s="5">
+      <c r="G28" s="7">
+        <v>0</v>
+      </c>
+      <c r="H28" s="7">
+        <v>0</v>
+      </c>
+      <c r="I28" s="7">
         <v>10490000</v>
       </c>
-      <c r="J28" s="5">
-        <v>0</v>
-      </c>
-      <c r="K28" s="5">
+      <c r="J28" s="7">
+        <v>0</v>
+      </c>
+      <c r="K28" s="7">
         <v>9</v>
       </c>
-      <c r="L28" s="5">
+      <c r="L28" s="7">
         <v>10490000</v>
       </c>
-      <c r="M28" s="5">
+      <c r="M28" s="7">
         <v>94410000</v>
       </c>
     </row>
@@ -1630,31 +1636,31 @@
       <c r="D29" s="5">
         <v>10</v>
       </c>
-      <c r="E29" s="5">
-        <v>0</v>
-      </c>
-      <c r="F29" s="5">
+      <c r="E29" s="7">
+        <v>0</v>
+      </c>
+      <c r="F29" s="7">
         <v>12400000</v>
       </c>
-      <c r="G29" s="5">
-        <v>0</v>
-      </c>
-      <c r="H29" s="5">
-        <v>0</v>
-      </c>
-      <c r="I29" s="5">
+      <c r="G29" s="7">
+        <v>0</v>
+      </c>
+      <c r="H29" s="7">
+        <v>0</v>
+      </c>
+      <c r="I29" s="7">
         <v>12400000</v>
       </c>
-      <c r="J29" s="5">
-        <v>0</v>
-      </c>
-      <c r="K29" s="5">
-        <v>10</v>
-      </c>
-      <c r="L29" s="5">
+      <c r="J29" s="7">
+        <v>0</v>
+      </c>
+      <c r="K29" s="7">
+        <v>10</v>
+      </c>
+      <c r="L29" s="7">
         <v>12400000</v>
       </c>
-      <c r="M29" s="5">
+      <c r="M29" s="7">
         <v>124000000</v>
       </c>
     </row>
@@ -1671,31 +1677,31 @@
       <c r="D30" s="5">
         <v>10</v>
       </c>
-      <c r="E30" s="5">
-        <v>0</v>
-      </c>
-      <c r="F30" s="5">
+      <c r="E30" s="7">
+        <v>0</v>
+      </c>
+      <c r="F30" s="7">
         <v>13990000</v>
       </c>
-      <c r="G30" s="5">
-        <v>0</v>
-      </c>
-      <c r="H30" s="5">
-        <v>0</v>
-      </c>
-      <c r="I30" s="5">
+      <c r="G30" s="7">
+        <v>0</v>
+      </c>
+      <c r="H30" s="7">
+        <v>0</v>
+      </c>
+      <c r="I30" s="7">
         <v>13990000</v>
       </c>
-      <c r="J30" s="5">
-        <v>0</v>
-      </c>
-      <c r="K30" s="5">
-        <v>10</v>
-      </c>
-      <c r="L30" s="5">
+      <c r="J30" s="7">
+        <v>0</v>
+      </c>
+      <c r="K30" s="7">
+        <v>10</v>
+      </c>
+      <c r="L30" s="7">
         <v>13990000</v>
       </c>
-      <c r="M30" s="5">
+      <c r="M30" s="7">
         <v>139900000</v>
       </c>
     </row>
@@ -1712,31 +1718,31 @@
       <c r="D31" s="5">
         <v>10</v>
       </c>
-      <c r="E31" s="5">
-        <v>0</v>
-      </c>
-      <c r="F31" s="5">
+      <c r="E31" s="7">
+        <v>0</v>
+      </c>
+      <c r="F31" s="7">
         <v>11690000</v>
       </c>
-      <c r="G31" s="5">
-        <v>0</v>
-      </c>
-      <c r="H31" s="5">
-        <v>0</v>
-      </c>
-      <c r="I31" s="5">
+      <c r="G31" s="7">
+        <v>0</v>
+      </c>
+      <c r="H31" s="7">
+        <v>0</v>
+      </c>
+      <c r="I31" s="7">
         <v>11690000</v>
       </c>
-      <c r="J31" s="5">
-        <v>0</v>
-      </c>
-      <c r="K31" s="5">
-        <v>10</v>
-      </c>
-      <c r="L31" s="5">
+      <c r="J31" s="7">
+        <v>0</v>
+      </c>
+      <c r="K31" s="7">
+        <v>10</v>
+      </c>
+      <c r="L31" s="7">
         <v>11690000</v>
       </c>
-      <c r="M31" s="5">
+      <c r="M31" s="7">
         <v>116900000</v>
       </c>
     </row>
@@ -1753,31 +1759,31 @@
       <c r="D32" s="5">
         <v>0</v>
       </c>
-      <c r="E32" s="5">
-        <v>0</v>
-      </c>
-      <c r="F32" s="5">
+      <c r="E32" s="7">
+        <v>0</v>
+      </c>
+      <c r="F32" s="7">
         <v>4790000</v>
       </c>
-      <c r="G32" s="5">
-        <v>0</v>
-      </c>
-      <c r="H32" s="5">
-        <v>0</v>
-      </c>
-      <c r="I32" s="5">
+      <c r="G32" s="7">
+        <v>0</v>
+      </c>
+      <c r="H32" s="7">
+        <v>0</v>
+      </c>
+      <c r="I32" s="7">
         <v>4790000</v>
       </c>
-      <c r="J32" s="5">
-        <v>0</v>
-      </c>
-      <c r="K32" s="5">
-        <v>0</v>
-      </c>
-      <c r="L32" s="5">
+      <c r="J32" s="7">
+        <v>0</v>
+      </c>
+      <c r="K32" s="7">
+        <v>0</v>
+      </c>
+      <c r="L32" s="7">
         <v>4790000</v>
       </c>
-      <c r="M32" s="5">
+      <c r="M32" s="7">
         <v>0</v>
       </c>
     </row>
@@ -1794,31 +1800,31 @@
       <c r="D33" s="5">
         <v>0</v>
       </c>
-      <c r="E33" s="5">
-        <v>0</v>
-      </c>
-      <c r="F33" s="5">
+      <c r="E33" s="7">
+        <v>0</v>
+      </c>
+      <c r="F33" s="7">
         <v>450000</v>
       </c>
-      <c r="G33" s="5">
-        <v>0</v>
-      </c>
-      <c r="H33" s="5">
-        <v>0</v>
-      </c>
-      <c r="I33" s="5">
+      <c r="G33" s="7">
+        <v>0</v>
+      </c>
+      <c r="H33" s="7">
+        <v>0</v>
+      </c>
+      <c r="I33" s="7">
         <v>450000</v>
       </c>
-      <c r="J33" s="5">
-        <v>0</v>
-      </c>
-      <c r="K33" s="5">
-        <v>0</v>
-      </c>
-      <c r="L33" s="5">
+      <c r="J33" s="7">
+        <v>0</v>
+      </c>
+      <c r="K33" s="7">
+        <v>0</v>
+      </c>
+      <c r="L33" s="7">
         <v>450000</v>
       </c>
-      <c r="M33" s="5">
+      <c r="M33" s="7">
         <v>0</v>
       </c>
     </row>
@@ -1835,31 +1841,31 @@
       <c r="D34" s="5">
         <v>0</v>
       </c>
-      <c r="E34" s="5">
-        <v>0</v>
-      </c>
-      <c r="F34" s="5">
+      <c r="E34" s="7">
+        <v>0</v>
+      </c>
+      <c r="F34" s="7">
         <v>430000</v>
       </c>
-      <c r="G34" s="5">
-        <v>0</v>
-      </c>
-      <c r="H34" s="5">
-        <v>0</v>
-      </c>
-      <c r="I34" s="5">
+      <c r="G34" s="7">
+        <v>0</v>
+      </c>
+      <c r="H34" s="7">
+        <v>0</v>
+      </c>
+      <c r="I34" s="7">
         <v>430000</v>
       </c>
-      <c r="J34" s="5">
-        <v>0</v>
-      </c>
-      <c r="K34" s="5">
-        <v>0</v>
-      </c>
-      <c r="L34" s="5">
+      <c r="J34" s="7">
+        <v>0</v>
+      </c>
+      <c r="K34" s="7">
+        <v>0</v>
+      </c>
+      <c r="L34" s="7">
         <v>430000</v>
       </c>
-      <c r="M34" s="5">
+      <c r="M34" s="7">
         <v>0</v>
       </c>
     </row>
@@ -1870,69 +1876,69 @@
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
-      <c r="E35" s="6">
+      <c r="E35" s="8">
         <v>5</v>
       </c>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6">
+      <c r="F35" s="8"/>
+      <c r="G35" s="8">
         <v>14600000</v>
       </c>
-      <c r="H35" s="6">
-        <v>0</v>
-      </c>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6">
-        <v>0</v>
-      </c>
-      <c r="K35" s="6">
+      <c r="H35" s="8">
+        <v>0</v>
+      </c>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8">
+        <v>0</v>
+      </c>
+      <c r="K35" s="8">
         <v>240</v>
       </c>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6">
+      <c r="L35" s="8"/>
+      <c r="M35" s="8">
         <v>3301200000</v>
       </c>
     </row>
     <row r="38" spans="1:13">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7" t="s">
+      <c r="A38" s="9"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7" t="s">
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7" t="s">
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="7"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
     </row>
     <row r="39" spans="1:13">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8" t="s">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8" t="s">
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8" t="s">
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="8"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
     </row>
   </sheetData>
   <mergeCells>

</xml_diff>